<commit_message>
adjusted some py and YELL R script
</commit_message>
<xml_diff>
--- a/Well Stats_NorthernRange.xlsx
+++ b/Well Stats_NorthernRange.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\NR wells\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRudolph\Documents\R Projects\wetland-wells\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6A26CC-8A65-49D0-B7BF-A52A9203FE00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC961C1E-CE75-4D8A-942A-8CFC8096C590}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29655" yWindow="-1725" windowWidth="18000" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="input for RockyR code" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Well</t>
   </si>
@@ -53,17 +54,59 @@
     <t>NR-BM305</t>
   </si>
   <si>
-    <t>NR-DC003</t>
-  </si>
-  <si>
     <t>NR-LT203</t>
+  </si>
+  <si>
+    <t>NR-DC3</t>
+  </si>
+  <si>
+    <t>NR-DC4</t>
+  </si>
+  <si>
+    <t>NR-IP128</t>
+  </si>
+  <si>
+    <t>NR-MB189</t>
+  </si>
+  <si>
+    <t>NR-SG180</t>
+  </si>
+  <si>
+    <t>NR-TF26</t>
+  </si>
+  <si>
+    <t>NR-IP1</t>
+  </si>
+  <si>
+    <t>NR-TL38</t>
+  </si>
+  <si>
+    <t>NR-TL299</t>
+  </si>
+  <si>
+    <t>NR-SV2</t>
+  </si>
+  <si>
+    <t>NR-TL34</t>
+  </si>
+  <si>
+    <t>NR-OR349</t>
+  </si>
+  <si>
+    <t>NR-LT74</t>
+  </si>
+  <si>
+    <t>NR-CR66</t>
+  </si>
+  <si>
+    <t>NR-WA320</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -73,15 +116,12 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -89,7 +129,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,12 +140,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -126,8 +160,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -143,6 +177,40 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="H2O&amp;BaroLogger_summer11"/>
+      <sheetName val="LoggerNames&amp;xy's"/>
+      <sheetName val="YNP_longtermLoggers_Fall11"/>
+      <sheetName val="Spg2012 well checks"/>
+      <sheetName val="Pressure scratch work"/>
+      <sheetName val="Fall2012 Well Checks"/>
+      <sheetName val="Fall2017_Summary"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2">
+        <row r="8">
+          <cell r="I8">
+            <v>22.5</v>
+          </cell>
+          <cell r="J8">
+            <v>6</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -411,10 +479,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -424,7 +493,7 @@
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,19 +527,16 @@
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4">
-        <v>0.33</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1.927</v>
+      <c r="B2" s="3">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1.883</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -478,17 +544,17 @@
       <c r="E2" s="3">
         <v>-0.3</v>
       </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1.901</v>
+      <c r="B3">
+        <f>SUM([1]YNP_longtermLoggers_Fall11!$I$8:$J$8)/100</f>
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.8859999999999999</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -496,17 +562,16 @@
       <c r="E3" s="3">
         <v>-0.3</v>
       </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1.865</v>
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2.3029999999999999</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -514,17 +579,16 @@
       <c r="E4" s="3">
         <v>-0.3</v>
       </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4">
-        <v>0.37</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1.4950000000000001</v>
+      <c r="B5" s="3">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.8680000000000001</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -532,7 +596,244 @@
       <c r="E5" s="3">
         <v>-0.3</v>
       </c>
-      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.2529999999999999</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.246</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.371</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.214</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2.1859999999999999</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.4179999999999999</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1.1639999999999999</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.185</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2.012</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.44</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.223</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.613</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1.5069999999999999</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1.032</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2.1819999999999999</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.441</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2.2109999999999999</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1.1220000000000001</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>-0.3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>